<commit_message>
some minor suntax fix
</commit_message>
<xml_diff>
--- a/spirale/Results.xlsx
+++ b/spirale/Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Object { size: 383616, visits: 5184, time: 563.2662282071011 }</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>Object { size: 49340, visits: 2467, time: 134.83914997232557 }</t>
+  </si>
+  <si>
+    <t>Func</t>
+  </si>
+  <si>
+    <t>Pa</t>
+  </si>
+  <si>
+    <t>Including type conversion</t>
+  </si>
+  <si>
+    <t>Object { size: 250410, visits: 2455, time: 2565.622217476026 }</t>
+  </si>
+  <si>
+    <t>Object { size: 46512, visits: 2448, time: 3946.8605084212986 }</t>
   </si>
 </sst>
 </file>
@@ -386,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -461,6 +476,28 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>